<commit_message>
latest commits on housing outcome
disregard the older files
</commit_message>
<xml_diff>
--- a/BoSClean/destination_value_counts.xlsx
+++ b/BoSClean/destination_value_counts.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Exit Destinations" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -25,58 +25,82 @@
     <t>Count</t>
   </si>
   <si>
+    <t>OC PATH</t>
+  </si>
+  <si>
+    <t>MC PATH</t>
+  </si>
+  <si>
+    <t>SPC</t>
+  </si>
+  <si>
+    <t>8319</t>
+  </si>
+  <si>
+    <t>Erin Park</t>
+  </si>
+  <si>
     <t>143</t>
   </si>
   <si>
+    <t>11495</t>
+  </si>
+  <si>
     <t>1371 FINAL</t>
   </si>
   <si>
-    <t>8319</t>
-  </si>
-  <si>
-    <t>11495</t>
-  </si>
-  <si>
-    <t>Erin Park</t>
-  </si>
-  <si>
-    <t>MC PATH</t>
-  </si>
-  <si>
-    <t>OC PATH</t>
-  </si>
-  <si>
-    <t>SPC</t>
-  </si>
-  <si>
     <t>Rental by client, with ongoing housing subsidy (HUD)</t>
   </si>
   <si>
+    <t>Staying or living with friends, temporary tenure (e.g., room, apartment, or house) (HUD)</t>
+  </si>
+  <si>
+    <t>Staying or living with friends, permanent tenure (HUD)</t>
+  </si>
+  <si>
+    <t>Rental by client, no ongoing housing subsidy (HUD)</t>
+  </si>
+  <si>
+    <t>Place not meant for habitation (e.g., a vehicle, an abandoned building, bus/train/subway station/airport or anywhere outside) (HUD)</t>
+  </si>
+  <si>
+    <t>Emergency shelter, including hotel or motel paid for with emergency shelter voucher, Host Home shelter (HUD)</t>
+  </si>
+  <si>
+    <t>Staying or living with family, permanent tenure (HUD)</t>
+  </si>
+  <si>
+    <t>Jail, prison, or juvenile detention facility (HUD)</t>
+  </si>
+  <si>
+    <t>Deceased (HUD)</t>
+  </si>
+  <si>
+    <t>Substance abuse treatment facility or detox center (HUD)</t>
+  </si>
+  <si>
+    <t>Transitional housing for homeless persons (including homeless youth) (HUD)</t>
+  </si>
+  <si>
+    <t>Staying or living with family, temporary tenure (e.g., room, apartment, or house) (HUD)</t>
+  </si>
+  <si>
+    <t>Hospital or other residential non-psychiatric medical facility (HUD)</t>
+  </si>
+  <si>
     <t>No exit interview completed (HUD)</t>
   </si>
   <si>
-    <t>Staying or living with family, permanent tenure (HUD)</t>
-  </si>
-  <si>
-    <t>Place not meant for habitation (e.g., a vehicle, an abandoned building, bus/train/subway station/airport or anywhere outside) (HUD)</t>
-  </si>
-  <si>
-    <t>Deceased (HUD)</t>
-  </si>
-  <si>
-    <t>Rental by client, no ongoing housing subsidy (HUD)</t>
-  </si>
-  <si>
-    <t>Staying or living with friends, permanent tenure (HUD)</t>
-  </si>
-  <si>
-    <t>Jail, prison, or juvenile detention facility (HUD)</t>
-  </si>
-  <si>
-    <t>Substance abuse treatment facility or detox center (HUD)</t>
-  </si>
-  <si>
-    <t>Emergency shelter, including hotel or motel paid for with emergency shelter voucher, Host Home shelter (HUD)</t>
+    <t>Other (HUD)</t>
+  </si>
+  <si>
+    <t>Hotel or motel paid for without emergency shelter voucher (HUD)</t>
+  </si>
+  <si>
+    <t>Data not collected (HUD)</t>
+  </si>
+  <si>
+    <t>Owned by client, no ongoing housing subsidy (HUD)</t>
   </si>
   <si>
     <t>Client doesn't know (HUD)</t>
@@ -88,34 +112,10 @@
     <t>Foster care home or foster care group home (HUD)</t>
   </si>
   <si>
-    <t>Staying or living with family, temporary tenure (e.g., room, apartment, or house) (HUD)</t>
-  </si>
-  <si>
     <t>Owned by client, with ongoing housing subsidy (HUD)</t>
   </si>
   <si>
     <t>Client prefers not to answer (HUD)</t>
-  </si>
-  <si>
-    <t>Hotel or motel paid for without emergency shelter voucher (HUD)</t>
-  </si>
-  <si>
-    <t>Staying or living with friends, temporary tenure (e.g., room, apartment, or house) (HUD)</t>
-  </si>
-  <si>
-    <t>Owned by client, no ongoing housing subsidy (HUD)</t>
-  </si>
-  <si>
-    <t>Transitional housing for homeless persons (including homeless youth) (HUD)</t>
-  </si>
-  <si>
-    <t>Other (HUD)</t>
-  </si>
-  <si>
-    <t>Data not collected (HUD)</t>
-  </si>
-  <si>
-    <t>Hospital or other residential non-psychiatric medical facility (HUD)</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -509,7 +509,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -520,7 +520,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -531,7 +531,7 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -553,7 +553,7 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -564,7 +564,7 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -575,7 +575,7 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -586,7 +586,7 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -597,7 +597,7 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -608,7 +608,7 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -619,62 +619,62 @@
         <v>22</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -682,10 +682,10 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C19">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -696,7 +696,7 @@
         <v>16</v>
       </c>
       <c r="C20">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -704,10 +704,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -715,285 +715,285 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C32">
-        <v>214</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C33">
-        <v>213</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C35">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C36">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C38">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1001,10 +1001,10 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1012,10 +1012,10 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C49">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1023,10 +1023,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C50">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1034,10 +1034,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1045,10 +1045,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C52">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1056,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -1067,10 +1067,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1078,7 +1078,7 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1089,7 +1089,7 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1097,24 +1097,24 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C57">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C58">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1122,10 +1122,10 @@
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1133,98 +1133,98 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C60">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C61">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64">
         <v>9</v>
-      </c>
-      <c r="B64" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1232,10 +1232,10 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C69">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1243,10 +1243,10 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1254,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -1265,7 +1265,7 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -1276,7 +1276,7 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C73">
         <v>1</v>

</xml_diff>